<commit_message>
Combo-boxes with pre-defined values
Combo-boxes with pre-defined values
</commit_message>
<xml_diff>
--- a/input_generico.xlsx
+++ b/input_generico.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/carvaa/Projects/ProposalCalculator/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ravanini/WorkDocs/workspace/ProposalCalculator/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15460"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14180"/>
   </bookViews>
   <sheets>
     <sheet name="Servers" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="88">
   <si>
     <t>Description</t>
   </si>
@@ -128,9 +128,6 @@
     <t>31/01/2017</t>
   </si>
   <si>
-    <t>standard</t>
-  </si>
-  <si>
     <t>Partial Upfront</t>
   </si>
   <si>
@@ -152,15 +149,6 @@
     <t>Linux</t>
   </si>
   <si>
-    <t>SQL Server Enterprise</t>
-  </si>
-  <si>
-    <t>SQL Std</t>
-  </si>
-  <si>
-    <t>SQL Web</t>
-  </si>
-  <si>
     <t>Server 1</t>
   </si>
   <si>
@@ -228,6 +216,84 @@
   </si>
   <si>
     <t>AFRESP</t>
+  </si>
+  <si>
+    <t>SAP Instance Type</t>
+  </si>
+  <si>
+    <t>US East (Ohio)</t>
+  </si>
+  <si>
+    <t>Standard</t>
+  </si>
+  <si>
+    <t>APPS</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>US West (Oregon)</t>
+  </si>
+  <si>
+    <t>Convertible</t>
+  </si>
+  <si>
+    <t>ANY_DB</t>
+  </si>
+  <si>
+    <t>SQLStandard</t>
+  </si>
+  <si>
+    <t>US West (N. California)</t>
+  </si>
+  <si>
+    <t>HANA_OLTP</t>
+  </si>
+  <si>
+    <t>SQLWeb</t>
+  </si>
+  <si>
+    <t>HANA_OLAP</t>
+  </si>
+  <si>
+    <t>SQLEnterprise</t>
+  </si>
+  <si>
+    <t>Asia Pacific (Mumbai)</t>
+  </si>
+  <si>
+    <t>Asia Pacific (Seoul)</t>
+  </si>
+  <si>
+    <t>Asia Pacific (Singapore)</t>
+  </si>
+  <si>
+    <t>Asia Pacific (Sydney)</t>
+  </si>
+  <si>
+    <t>Asia Pacific (Tokyo)</t>
+  </si>
+  <si>
+    <t>AWS GovCloud (US)</t>
+  </si>
+  <si>
+    <t>Canada (Central)</t>
+  </si>
+  <si>
+    <t>China (Beijing)</t>
+  </si>
+  <si>
+    <t>EU (Frankfurt)</t>
+  </si>
+  <si>
+    <t>EU (Ireland)</t>
+  </si>
+  <si>
+    <t>EU (London)</t>
+  </si>
+  <si>
+    <t>Valid Combinations for Purchasing Option</t>
   </si>
 </sst>
 </file>
@@ -237,10 +303,17 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -310,8 +383,15 @@
       <sz val="11"/>
       <name val="Calibri"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -324,8 +404,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor theme="0" tint="-0.14999847407452621"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="7">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -403,31 +495,113 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -438,7 +612,41 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="2" borderId="3" xfId="4" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="2" borderId="6" xfId="4" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -1575,9 +1783,9 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="G1:S6" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17">
-  <autoFilter ref="G1:S6"/>
-  <tableColumns count="13">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="G1:T17" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17">
+  <autoFilter ref="G1:T17"/>
+  <tableColumns count="14">
     <tableColumn id="1" name="Storage(GB)" dataDxfId="16"/>
     <tableColumn id="2" name="Volume Type" dataDxfId="15"/>
     <tableColumn id="3" name="IOPS"/>
@@ -1588,6 +1796,7 @@
     <tableColumn id="8" name="Offering Class" dataDxfId="11"/>
     <tableColumn id="9" name="Tenancy" dataDxfId="10"/>
     <tableColumn id="10" name="Operating System"/>
+    <tableColumn id="14" name="SAP Instance Type"/>
     <tableColumn id="11" name="Pre Installed S/W"/>
     <tableColumn id="12" name="Beginning" dataDxfId="9"/>
     <tableColumn id="13" name="End" dataDxfId="8"/>
@@ -1597,8 +1806,8 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="A1:F6" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
-  <autoFilter ref="A1:F6"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="A1:F17" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
+  <autoFilter ref="A1:F17"/>
   <tableColumns count="6">
     <tableColumn id="1" name="Description" dataDxfId="5"/>
     <tableColumn id="2" name="Region" dataDxfId="4"/>
@@ -1876,8 +2085,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
+      <selection activeCell="U2" sqref="U2:U1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1913,7 +2122,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="C1" s="7" t="s">
         <v>10</v>
@@ -1922,7 +2131,7 @@
         <v>5</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="F1" s="7" t="s">
         <v>1</v>
@@ -1964,10 +2173,10 @@
         <v>14</v>
       </c>
       <c r="S1" s="7" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="T1" s="7" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="U1" s="7" t="s">
         <v>28</v>
@@ -1981,10 +2190,10 @@
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="D2" s="2">
         <v>1</v>
@@ -2029,18 +2238,18 @@
         <v>30</v>
       </c>
       <c r="S2" s="2" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="T2" s="2" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="D3" s="2">
         <v>1</v>
@@ -2085,18 +2294,18 @@
         <v>30</v>
       </c>
       <c r="S3" s="2" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="T3" s="2" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="D4" s="2">
         <v>1</v>
@@ -2114,7 +2323,7 @@
         <v>500</v>
       </c>
       <c r="J4" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="L4">
         <v>250</v>
@@ -2138,18 +2347,18 @@
         <v>30</v>
       </c>
       <c r="S4" s="2" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="T4" s="2" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="D5" s="2">
         <v>1</v>
@@ -2167,7 +2376,7 @@
         <v>500</v>
       </c>
       <c r="J5" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="L5">
         <v>250</v>
@@ -2191,18 +2400,18 @@
         <v>30</v>
       </c>
       <c r="S5" s="2" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="T5" s="2" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="6" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="D6" s="2">
         <v>1</v>
@@ -2220,7 +2429,7 @@
         <v>500</v>
       </c>
       <c r="J6" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="L6">
         <v>250</v>
@@ -2244,18 +2453,18 @@
         <v>30</v>
       </c>
       <c r="S6" s="2" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="T6" s="2" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="7" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="D7" s="2">
         <v>1</v>
@@ -2273,7 +2482,7 @@
         <v>500</v>
       </c>
       <c r="J7" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="L7">
         <v>250</v>
@@ -2297,18 +2506,18 @@
         <v>30</v>
       </c>
       <c r="S7" s="2" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="T7" s="2" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="8" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="D8" s="2">
         <v>1</v>
@@ -2326,7 +2535,7 @@
         <v>500</v>
       </c>
       <c r="J8" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="L8">
         <v>250</v>
@@ -2350,10 +2559,10 @@
         <v>30</v>
       </c>
       <c r="S8" s="2" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="T8" s="2" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="U8"/>
     </row>
@@ -2462,6 +2671,66 @@
   <tableParts count="1">
     <tablePart r:id="rId1"/>
   </tableParts>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="9">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Help!$B$2:$B$17</xm:f>
+          </x14:formula1>
+          <xm:sqref>C2:C1048576</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Help!$H$2:$H$6</xm:f>
+          </x14:formula1>
+          <xm:sqref>J2:J1048576</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Help!$K$2:$K$3</xm:f>
+          </x14:formula1>
+          <xm:sqref>M2:M1048576</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Help!$L$2:$L$3</xm:f>
+          </x14:formula1>
+          <xm:sqref>N2:N1048576</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Help!$M$2:$M$4</xm:f>
+          </x14:formula1>
+          <xm:sqref>O2:O1048576</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Help!$N$2:$N$3</xm:f>
+          </x14:formula1>
+          <xm:sqref>P2:P1048576</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Help!$O$2:$O$3</xm:f>
+          </x14:formula1>
+          <xm:sqref>Q2:Q1048576</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Help!$P$2:$P$5</xm:f>
+          </x14:formula1>
+          <xm:sqref>R2:R1048576</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Help!$R$2:$R$5</xm:f>
+          </x14:formula1>
+          <xm:sqref>U2:U1048576</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -2492,7 +2761,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="13" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B2" s="14">
         <v>0</v>
@@ -2567,13 +2836,13 @@
         <v>8</v>
       </c>
       <c r="D1" s="16" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="E1" s="16" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="F1" s="17" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -2600,18 +2869,18 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S17"/>
+  <dimension ref="A1:T29"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="O2" sqref="O2"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="12.33203125" style="2" customWidth="1"/>
     <col min="2" max="2" width="20.83203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.83203125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="6.83203125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="13.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.5" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="18.5" style="1" customWidth="1"/>
     <col min="6" max="6" width="10.1640625" style="4" customWidth="1"/>
     <col min="7" max="7" width="12.6640625" style="2" customWidth="1"/>
@@ -2630,7 +2899,7 @@
     <col min="20" max="16384" width="8.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:20" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -2680,21 +2949,24 @@
         <v>14</v>
       </c>
       <c r="Q1" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="R1" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="R1" s="10" t="s">
+      <c r="S1" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="S1" s="9" t="s">
+      <c r="T1" s="9" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:20" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>22</v>
+        <v>63</v>
       </c>
       <c r="C2" s="5">
         <v>1</v>
@@ -2724,13 +2996,13 @@
         <v>23</v>
       </c>
       <c r="L2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="M2" t="s">
         <v>25</v>
       </c>
       <c r="N2" t="s">
-        <v>32</v>
+        <v>64</v>
       </c>
       <c r="O2" s="5" t="s">
         <v>13</v>
@@ -2739,18 +3011,21 @@
         <v>30</v>
       </c>
       <c r="Q2" t="s">
-        <v>40</v>
-      </c>
-      <c r="R2" s="5" t="s">
-        <v>31</v>
+        <v>65</v>
+      </c>
+      <c r="R2" t="s">
+        <v>66</v>
       </c>
       <c r="S2" s="5" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T2" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
-        <v>44</v>
+        <v>67</v>
       </c>
       <c r="C3" s="2">
         <v>5</v>
@@ -2762,7 +3037,7 @@
         <v>100</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="I3">
         <v>1000</v>
@@ -2771,100 +3046,361 @@
         <v>0</v>
       </c>
       <c r="K3" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="L3" t="s">
         <v>24</v>
       </c>
       <c r="M3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="N3" t="s">
-        <v>26</v>
+        <v>68</v>
       </c>
       <c r="O3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="P3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="Q3" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
+        <v>69</v>
+      </c>
+      <c r="R3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B4" s="2" t="s">
+        <v>71</v>
+      </c>
       <c r="G4" s="2">
         <v>100</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="M4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="P4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="Q4" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
+        <v>72</v>
+      </c>
+      <c r="R4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B5" s="2" t="s">
+        <v>22</v>
+      </c>
       <c r="G5" s="2">
         <v>500</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="P5" t="s">
-        <v>39</v>
-      </c>
-      <c r="Q5"/>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.2">
+        <v>38</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>74</v>
+      </c>
+      <c r="R5" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B6" s="2" t="s">
+        <v>76</v>
+      </c>
       <c r="G6" s="2">
         <v>500</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="Q6"/>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="Q7"/>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.2">
+        <v>44</v>
+      </c>
+      <c r="R6"/>
+    </row>
+    <row r="7" spans="1:20" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B7" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="R7"/>
+    </row>
+    <row r="8" spans="1:20" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B8" s="2" t="s">
+        <v>78</v>
+      </c>
       <c r="P8"/>
       <c r="Q8"/>
-    </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="R8"/>
+    </row>
+    <row r="9" spans="1:20" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B9" s="2" t="s">
+        <v>79</v>
+      </c>
       <c r="P9"/>
-    </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="Q9"/>
+      <c r="R9" s="1"/>
+    </row>
+    <row r="10" spans="1:20" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B10" s="2" t="s">
+        <v>80</v>
+      </c>
       <c r="P10"/>
-    </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="Q10"/>
+      <c r="R10" s="1"/>
+    </row>
+    <row r="11" spans="1:20" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B11" s="2" t="s">
+        <v>81</v>
+      </c>
       <c r="P11"/>
-    </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="Q11"/>
+      <c r="R11" s="1"/>
+    </row>
+    <row r="12" spans="1:20" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B12" s="2" t="s">
+        <v>82</v>
+      </c>
       <c r="P12"/>
-    </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="Q12"/>
+      <c r="R12" s="1"/>
+    </row>
+    <row r="13" spans="1:20" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B13" s="2" t="s">
+        <v>83</v>
+      </c>
       <c r="P13"/>
-    </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="Q13"/>
+      <c r="R13" s="1"/>
+    </row>
+    <row r="14" spans="1:20" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B14" s="2" t="s">
+        <v>84</v>
+      </c>
       <c r="P14"/>
-    </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="Q14"/>
+      <c r="R14" s="1"/>
+    </row>
+    <row r="15" spans="1:20" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B15" s="2" t="s">
+        <v>85</v>
+      </c>
       <c r="P15"/>
-    </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="Q15"/>
+      <c r="R15" s="1"/>
+    </row>
+    <row r="16" spans="1:20" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B16" s="2" t="s">
+        <v>86</v>
+      </c>
       <c r="P16"/>
-    </row>
-    <row r="17" spans="16:16" x14ac:dyDescent="0.2">
+      <c r="Q16"/>
+      <c r="R16" s="1"/>
+    </row>
+    <row r="17" spans="1:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B17" s="2" t="s">
+        <v>40</v>
+      </c>
       <c r="P17"/>
+      <c r="Q17"/>
+      <c r="R17" s="1"/>
+    </row>
+    <row r="18" spans="1:18" ht="14" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="R18" s="1"/>
+    </row>
+    <row r="19" spans="1:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="23" t="s">
+        <v>87</v>
+      </c>
+      <c r="B19" s="24"/>
+      <c r="C19" s="24"/>
+      <c r="D19" s="25"/>
+      <c r="R19" s="1"/>
+    </row>
+    <row r="20" spans="1:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="B20" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="C20" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="D20" s="26" t="s">
+        <v>17</v>
+      </c>
+      <c r="R20" s="1"/>
+    </row>
+    <row r="21" spans="1:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="27" t="s">
+        <v>45</v>
+      </c>
+      <c r="B21" s="28"/>
+      <c r="C21" s="29"/>
+      <c r="D21" s="30"/>
+      <c r="R21" s="1"/>
+    </row>
+    <row r="22" spans="1:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="31" t="s">
+        <v>23</v>
+      </c>
+      <c r="B22" s="32" t="s">
+        <v>34</v>
+      </c>
+      <c r="C22" s="32" t="s">
+        <v>25</v>
+      </c>
+      <c r="D22" s="33" t="s">
+        <v>64</v>
+      </c>
+      <c r="R22" s="1"/>
+    </row>
+    <row r="23" spans="1:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="34" t="s">
+        <v>23</v>
+      </c>
+      <c r="B23" s="35" t="s">
+        <v>34</v>
+      </c>
+      <c r="C23" s="36" t="s">
+        <v>32</v>
+      </c>
+      <c r="D23" s="37" t="s">
+        <v>64</v>
+      </c>
+      <c r="R23" s="1"/>
+    </row>
+    <row r="24" spans="1:18" s="42" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="38" t="s">
+        <v>23</v>
+      </c>
+      <c r="B24" s="39" t="s">
+        <v>34</v>
+      </c>
+      <c r="C24" s="32" t="s">
+        <v>33</v>
+      </c>
+      <c r="D24" s="33" t="s">
+        <v>64</v>
+      </c>
+      <c r="E24" s="40"/>
+      <c r="F24" s="41"/>
+      <c r="I24" s="43"/>
+      <c r="K24" s="40"/>
+      <c r="L24" s="40"/>
+      <c r="M24" s="40"/>
+      <c r="N24" s="40"/>
+      <c r="O24" s="40"/>
+      <c r="P24" s="40"/>
+      <c r="Q24" s="40"/>
+      <c r="R24" s="40"/>
+    </row>
+    <row r="25" spans="1:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="34" t="s">
+        <v>23</v>
+      </c>
+      <c r="B25" s="44" t="s">
+        <v>24</v>
+      </c>
+      <c r="C25" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="D25" s="37" t="s">
+        <v>64</v>
+      </c>
+      <c r="R25" s="1"/>
+    </row>
+    <row r="26" spans="1:18" s="42" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="38" t="s">
+        <v>23</v>
+      </c>
+      <c r="B26" s="42" t="s">
+        <v>24</v>
+      </c>
+      <c r="C26" s="42" t="s">
+        <v>33</v>
+      </c>
+      <c r="D26" s="33" t="s">
+        <v>64</v>
+      </c>
+      <c r="E26" s="40"/>
+      <c r="F26" s="41"/>
+      <c r="I26" s="43"/>
+      <c r="K26" s="40"/>
+      <c r="L26" s="40"/>
+      <c r="M26" s="40"/>
+      <c r="N26" s="40"/>
+      <c r="O26" s="40"/>
+      <c r="P26" s="40"/>
+      <c r="Q26" s="40"/>
+      <c r="R26" s="40"/>
+    </row>
+    <row r="27" spans="1:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="34" t="s">
+        <v>23</v>
+      </c>
+      <c r="B27" s="44" t="s">
+        <v>24</v>
+      </c>
+      <c r="C27" s="45" t="s">
+        <v>25</v>
+      </c>
+      <c r="D27" s="46" t="s">
+        <v>68</v>
+      </c>
+      <c r="R27" s="1"/>
+    </row>
+    <row r="28" spans="1:18" s="42" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="38" t="s">
+        <v>23</v>
+      </c>
+      <c r="B28" s="42" t="s">
+        <v>24</v>
+      </c>
+      <c r="C28" s="32" t="s">
+        <v>32</v>
+      </c>
+      <c r="D28" s="33" t="s">
+        <v>68</v>
+      </c>
+      <c r="E28" s="40"/>
+      <c r="F28" s="41"/>
+      <c r="I28" s="43"/>
+      <c r="K28" s="40"/>
+      <c r="L28" s="40"/>
+      <c r="M28" s="40"/>
+      <c r="N28" s="40"/>
+      <c r="O28" s="40"/>
+      <c r="P28" s="40"/>
+      <c r="Q28" s="40"/>
+      <c r="R28" s="40"/>
+    </row>
+    <row r="29" spans="1:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="47" t="s">
+        <v>23</v>
+      </c>
+      <c r="B29" s="48" t="s">
+        <v>24</v>
+      </c>
+      <c r="C29" s="49" t="s">
+        <v>33</v>
+      </c>
+      <c r="D29" s="50" t="s">
+        <v>68</v>
+      </c>
+      <c r="R29" s="1"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A19:D19"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="2">
     <tablePart r:id="rId1"/>

</xml_diff>